<commit_message>
Allowing exception file from EHS to be processed
data file is put in ENV['CAMPUS_ACCESS_DIRECTORY']
</commit_message>
<xml_diff>
--- a/spec/fixtures/access.xlsx
+++ b/spec/fixtures/access.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/projects/marc_liberation/spec/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colec/projects/marc_liberation/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD49E71-412F-0D47-92B3-145A57E986FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B478B7-C4A7-D440-A4D3-C61267828628}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35580" yWindow="-3020" windowWidth="27640" windowHeight="16940" xr2:uid="{02627929-8C5B-4049-BABC-8D7E9666C1E0}"/>
+    <workbookView xWindow="6520" yWindow="2640" windowWidth="27640" windowHeight="16940" xr2:uid="{02627929-8C5B-4049-BABC-8D7E9666C1E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -492,6 +492,9 @@
     <xf numFmtId="165" fontId="5" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -520,9 +523,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -889,7 +889,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -898,48 +898,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="17"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="21" t="s">
+      <c r="A1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="22">
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="23">
         <v>44089</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="23"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="24"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="24">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="25">
         <v>0.57291665999999997</v>
       </c>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="25"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="26"/>
     </row>
     <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1005,8 +1005,8 @@
       <c r="G5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="30">
-        <v>10001111</v>
+      <c r="H5" s="13">
+        <v>10001112</v>
       </c>
       <c r="I5" s="6">
         <v>44041.429062499999</v>
@@ -1120,7 +1120,7 @@
         <v>15</v>
       </c>
       <c r="H8" s="8">
-        <v>10001111</v>
+        <v>10001113</v>
       </c>
       <c r="I8" s="9">
         <v>44079.168368049999</v>
@@ -1158,7 +1158,7 @@
         <v>15</v>
       </c>
       <c r="H9" s="8">
-        <v>10001111</v>
+        <v>10001114</v>
       </c>
       <c r="I9" s="9">
         <v>44036.676192129999</v>
@@ -1196,7 +1196,7 @@
         <v>15</v>
       </c>
       <c r="H10" s="8">
-        <v>10001111</v>
+        <v>10001115</v>
       </c>
       <c r="I10" s="9">
         <v>44036.690694440003</v>
@@ -1234,7 +1234,7 @@
         <v>15</v>
       </c>
       <c r="H11" s="8">
-        <v>10001111</v>
+        <v>10001116</v>
       </c>
       <c r="I11" s="9">
         <v>44041.418657399998</v>
@@ -1264,58 +1264,58 @@
       <c r="H12" s="12">
         <v>6505</v>
       </c>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="29"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="23"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="24"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="25"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="26"/>
     </row>
     <row r="15" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15" t="s">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="16"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
Allowing exception file from EHS to be processed (#949)
data file is put in ENV['CAMPUS_ACCESS_DIRECTORY']
</commit_message>
<xml_diff>
--- a/spec/fixtures/access.xlsx
+++ b/spec/fixtures/access.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/projects/marc_liberation/spec/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colec/projects/marc_liberation/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD49E71-412F-0D47-92B3-145A57E986FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B478B7-C4A7-D440-A4D3-C61267828628}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35580" yWindow="-3020" windowWidth="27640" windowHeight="16940" xr2:uid="{02627929-8C5B-4049-BABC-8D7E9666C1E0}"/>
+    <workbookView xWindow="6520" yWindow="2640" windowWidth="27640" windowHeight="16940" xr2:uid="{02627929-8C5B-4049-BABC-8D7E9666C1E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -492,6 +492,9 @@
     <xf numFmtId="165" fontId="5" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -520,9 +523,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -889,7 +889,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -898,48 +898,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="17"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="21" t="s">
+      <c r="A1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="22">
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="23">
         <v>44089</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="23"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="24"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="24">
+      <c r="A2" s="20"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="25">
         <v>0.57291665999999997</v>
       </c>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="25"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="26"/>
     </row>
     <row r="3" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1005,8 +1005,8 @@
       <c r="G5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="30">
-        <v>10001111</v>
+      <c r="H5" s="13">
+        <v>10001112</v>
       </c>
       <c r="I5" s="6">
         <v>44041.429062499999</v>
@@ -1120,7 +1120,7 @@
         <v>15</v>
       </c>
       <c r="H8" s="8">
-        <v>10001111</v>
+        <v>10001113</v>
       </c>
       <c r="I8" s="9">
         <v>44079.168368049999</v>
@@ -1158,7 +1158,7 @@
         <v>15</v>
       </c>
       <c r="H9" s="8">
-        <v>10001111</v>
+        <v>10001114</v>
       </c>
       <c r="I9" s="9">
         <v>44036.676192129999</v>
@@ -1196,7 +1196,7 @@
         <v>15</v>
       </c>
       <c r="H10" s="8">
-        <v>10001111</v>
+        <v>10001115</v>
       </c>
       <c r="I10" s="9">
         <v>44036.690694440003</v>
@@ -1234,7 +1234,7 @@
         <v>15</v>
       </c>
       <c r="H11" s="8">
-        <v>10001111</v>
+        <v>10001116</v>
       </c>
       <c r="I11" s="9">
         <v>44041.418657399998</v>
@@ -1264,58 +1264,58 @@
       <c r="H12" s="12">
         <v>6505</v>
       </c>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="29"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="23"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="24"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="25"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="26"/>
     </row>
     <row r="15" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15" t="s">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="16"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>